<commit_message>
added one group files
</commit_message>
<xml_diff>
--- a/benchmarks/gradient_simulations-90.0-days.xlsx
+++ b/benchmarks/gradient_simulations-90.0-days.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>heuristic</t>
   </si>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,7 +450,7 @@
         <v>0.5</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="E2">
         <v>3000</v>
@@ -462,45 +462,13 @@
         <v>10</v>
       </c>
       <c r="H2">
-        <v>58003134915.10947</v>
+        <v>28917147085.4152</v>
       </c>
       <c r="I2">
-        <v>47113.12199081807</v>
+        <v>6791.110624416735</v>
       </c>
       <c r="J2">
-        <v>54212606193.17973</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>0.5</v>
-      </c>
-      <c r="D3">
-        <v>1000000</v>
-      </c>
-      <c r="E3">
-        <v>3000</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>50132978458.96886</v>
-      </c>
-      <c r="I3">
-        <v>12808.01833921698</v>
-      </c>
-      <c r="J3">
-        <v>36290462531.10361</v>
+        <v>21770108661.10713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>